<commit_message>
Custom Exceptions and Encoding Decoding
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbavisa\eclipse-workspace\seleniumUIEndToEnd\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C922CD-2234-42CB-B800-A2CA0759C925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C3CEAC-37FD-4B09-95A6-92443B9FED13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNNER" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
   <si>
     <t>testname</t>
   </si>
@@ -40,82 +40,79 @@
     <t>count</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>amazonTest</t>
+  </si>
+  <si>
+    <t>To check whether amazon  test is executed</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>menutext</t>
+  </si>
+  <si>
+    <t>Laptops</t>
+  </si>
+  <si>
     <t>loginLogoutTest</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>sagar</t>
+  </si>
+  <si>
+    <t>testing mini bytes</t>
+  </si>
+  <si>
     <t>newTest</t>
   </si>
   <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>subscribe</t>
+  </si>
+  <si>
     <t>To check whether user can successfully login and logout</t>
   </si>
   <si>
     <t>To check whether test is executed</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>sagar</t>
-  </si>
-  <si>
-    <t>testing mini bytes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>subscribe</t>
-  </si>
-  <si>
-    <t>admin12</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>amazonTest</t>
-  </si>
-  <si>
-    <t>To check whether amazon  test is executed</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>menutext</t>
-  </si>
-  <si>
-    <t>Laptops</t>
+    <t>YWRtaW4xMjM=</t>
   </si>
 </sst>
 </file>
@@ -189,13 +186,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,71 +486,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -565,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26EDFCB-1FEE-4748-AF78-3D89E47DC17E}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,150 +574,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>